<commit_message>
feat: Add content viewer, streaming download, and fix task form logic
</commit_message>
<xml_diff>
--- a/qed_utility/static/assets/bulk_upload.xlsx
+++ b/qed_utility/static/assets/bulk_upload.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QACA\QED Portal\qed_utility\qed_utility\static\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EAEA2BE-6938-4CD1-98BD-FE664B5B0B2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB673F8E-068C-4E35-AA79-4091E601B65D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B2849511-E770-44CF-B8E2-2FA2CACB67FC}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>qacajobid</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>surveytargetdate</t>
+  </si>
+  <si>
+    <t>type</t>
   </si>
 </sst>
 </file>
@@ -447,80 +450,82 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{319B252E-7314-480D-89B9-1B8D60620530}">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:K2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="14.90625" customWidth="1"/>
-    <col min="7" max="7" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.90625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.08984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.90625" customWidth="1"/>
+    <col min="8" max="8" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.90625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.08984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A2" s="2"/>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="3"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="2"/>
       <c r="K2" s="3"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" s="2"/>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -529,10 +534,11 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
-      <c r="J3" s="3"/>
+      <c r="J3" s="2"/>
       <c r="K3" s="3"/>
-      <c r="L3" s="2"/>
+      <c r="L3" s="3"/>
       <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix task submission 500 error, improve bulk upload validation, update dashboard permissions and redirect
</commit_message>
<xml_diff>
--- a/qed_utility/static/assets/bulk_upload.xlsx
+++ b/qed_utility/static/assets/bulk_upload.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QACA\QED Portal\qed_utility\qed_utility\static\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB673F8E-068C-4E35-AA79-4091E601B65D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B969C26-827E-4502-BBAC-8A647B5FA1E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B2849511-E770-44CF-B8E2-2FA2CACB67FC}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>qacajobid</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>type</t>
+  </si>
+  <si>
+    <t>assignsurveycoordinator</t>
   </si>
 </sst>
 </file>
@@ -450,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{319B252E-7314-480D-89B9-1B8D60620530}">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -466,7 +469,7 @@
     <col min="14" max="14" width="10.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -509,8 +512,11 @@
       <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -525,7 +531,7 @@
       <c r="M2" s="2"/>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>

</xml_diff>